<commit_message>
Archivo unificado de datos y documentacion del mismo
Se creo el archivo 'Universidad.xlsx en el directorio de assets por defecto.
La idea es que las distintas caracteristicas iniciales del problema se encuentren en un sheet con este mismo formato, siempre.
A partir de los nombres de columnas establecitos aqui, se refactorizara parte del codigo del objeto universidad para que sea mas ligeble y no haga referencias dinamicas al nombre de columna. Tambien un archivo de estos, en blanco, sera lo que se le dara al usuario para llenar o importar
</commit_message>
<xml_diff>
--- a/src/assets/edificios_default/edificios.xlsx
+++ b/src/assets/edificios_default/edificios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t xml:space="preserve">Nombre del Edificio</t>
   </si>
@@ -49,10 +49,16 @@
     <t xml:space="preserve">Anasagasti 1</t>
   </si>
   <si>
-    <t xml:space="preserve">"9:00-18:00" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"12:00-21:00" </t>
+    <t xml:space="preserve">9:00-18:00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:00-21:00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00-18:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:00-21:00</t>
   </si>
   <si>
     <t xml:space="preserve">CERRADO</t>
@@ -61,7 +67,7 @@
     <t xml:space="preserve">Anasagasti 2</t>
   </si>
   <si>
-    <t xml:space="preserve">"9:00-12:00" </t>
+    <t xml:space="preserve">9:00-12:00</t>
   </si>
   <si>
     <t xml:space="preserve">Mitre 1</t>
@@ -178,7 +184,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -223,50 +229,50 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -275,19 +281,19 @@
         <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="47.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>